<commit_message>
Add new flavour for TCA9517 i2c buffer
</commit_message>
<xml_diff>
--- a/iot2000/CAD/BOM.xlsx
+++ b/iot2000/CAD/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cchapellier/home/Projets/Air Liquide/Predictable Farm/Commande nouvelles cartes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cchapellier/home/www/PF_embedded-software/iot2000/CAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
   <si>
     <t>Qté</t>
   </si>
@@ -225,6 +225,18 @@
   </si>
   <si>
     <t>594-MBB02070C1004FCT</t>
+  </si>
+  <si>
+    <t>538-22-28-4205</t>
+  </si>
+  <si>
+    <t>Headers 20P - to break away</t>
+  </si>
+  <si>
+    <t>22-28-4205</t>
+  </si>
+  <si>
+    <t>Header breakaway 20P 1R</t>
   </si>
 </sst>
 </file>
@@ -234,7 +246,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -265,6 +277,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -286,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -303,6 +322,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,7 +702,7 @@
         <v>0.15</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I13" si="0">H3*B3</f>
+        <f t="shared" ref="I3:I14" si="0">H3*B3</f>
         <v>0.15</v>
       </c>
     </row>
@@ -986,35 +1006,65 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="4">
-        <f>SUM(I12:I13,I4:I9,I2)</f>
-        <v>18.286000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H16" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8360000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="4">
+        <f>SUM(I4:I14,I2)</f>
+        <v>20.727999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
         <v>53</v>
       </c>
-      <c r="I16" s="4">
-        <f>I11+I10+I3</f>
-        <v>0.75600000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H17" t="s">
+      <c r="I21" s="4">
+        <f>I3</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="22" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="8">
-        <f>SUM(I2:I13)</f>
-        <v>19.042000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="J18" s="4"/>
+      <c r="I22" s="8">
+        <f>SUM(I2:I14)</f>
+        <v>20.878</v>
+      </c>
+    </row>
+    <row r="23" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="J23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Replace 1.2M resistor with 470k
</commit_message>
<xml_diff>
--- a/iot2000/CAD/BOM.xlsx
+++ b/iot2000/CAD/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="-15120" windowWidth="22640" windowHeight="12820" tabRatio="500"/>
+    <workbookView xWindow="-5720" yWindow="-19380" windowWidth="22640" windowHeight="12820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="80">
   <si>
     <t>Qté</t>
   </si>
@@ -107,12 +107,6 @@
     <t>JST</t>
   </si>
   <si>
-    <t>R3, R4</t>
-  </si>
-  <si>
-    <t>4.7 k 5%</t>
-  </si>
-  <si>
     <t>1 M 5%</t>
   </si>
   <si>
@@ -125,9 +119,6 @@
     <t>Vishay</t>
   </si>
   <si>
-    <t>1.2M 1%</t>
-  </si>
-  <si>
     <t>C315C102J3H5TA91707301</t>
   </si>
   <si>
@@ -200,12 +191,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>594-MBB02070C1204FCT</t>
-  </si>
-  <si>
-    <t>MBB02070C1204FCT00</t>
-  </si>
-  <si>
     <t>100V, 0.1 nF (100pf)</t>
   </si>
   <si>
@@ -215,12 +200,6 @@
     <t>594-K101J15C0GH53H5H</t>
   </si>
   <si>
-    <t>MBB02070C4701FCT00</t>
-  </si>
-  <si>
-    <t>594-MBB02070C4701FCT</t>
-  </si>
-  <si>
     <t>MBB02070C1004FCT00</t>
   </si>
   <si>
@@ -237,6 +216,57 @@
   </si>
   <si>
     <t>Header breakaway 20P 1R</t>
+  </si>
+  <si>
+    <t>IC5</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>TCA9517</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>Level-Shifting I2C Bus Repeater</t>
+  </si>
+  <si>
+    <t>595-TCA9517DR</t>
+  </si>
+  <si>
+    <t>C315C103M5U5TA</t>
+  </si>
+  <si>
+    <t>80-C315C103M5U</t>
+  </si>
+  <si>
+    <t>50V 0.01µF</t>
+  </si>
+  <si>
+    <t>Digikey (ou RS)</t>
+  </si>
+  <si>
+    <t>470k 1%</t>
+  </si>
+  <si>
+    <t>MBB02070C4703FCT00</t>
+  </si>
+  <si>
+    <t>594-MBB02070C4703FCT</t>
+  </si>
+  <si>
+    <t>MBB02070C1002FCT00</t>
+  </si>
+  <si>
+    <t>10k 1%</t>
+  </si>
+  <si>
+    <t>594-MBB02070C1002FCT</t>
+  </si>
+  <si>
+    <t>R3, R4, R11, R12</t>
   </si>
 </sst>
 </file>
@@ -246,7 +276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -284,6 +314,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -305,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -323,6 +359,17 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,6 +660,7 @@
     <col min="3" max="3" width="24.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="29.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="22.33203125" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
@@ -634,16 +682,16 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -654,19 +702,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H2" s="4">
         <v>0.46700000000000003</v>
@@ -684,25 +732,25 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H3">
         <v>0.15</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I14" si="0">H3*B3</f>
+        <f t="shared" ref="I3:I16" si="0">H3*B3</f>
         <v>0.15</v>
       </c>
     </row>
@@ -723,10 +771,10 @@
         <v>13</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H4" s="4">
         <v>1.23</v>
@@ -753,10 +801,10 @@
         <v>23</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H5" s="4">
         <v>0.68899999999999995</v>
@@ -774,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -783,10 +831,10 @@
         <v>21</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H6" s="4">
         <v>0.76300000000000001</v>
@@ -813,10 +861,10 @@
         <v>10</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H7" s="4">
         <v>11.21</v>
@@ -834,19 +882,19 @@
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
       <c r="F8" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H8" s="4">
         <v>0.77900000000000003</v>
@@ -864,19 +912,19 @@
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="H9" s="4">
         <v>8.2000000000000003E-2</v>
@@ -893,178 +941,238 @@
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0.09</v>
+      <c r="C10" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="15">
+        <v>9.4E-2</v>
       </c>
       <c r="I10" s="4">
         <f t="shared" si="0"/>
-        <v>0.18</v>
+        <v>0.188</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0.21299999999999999</v>
+        <v>41</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="17">
+        <v>9.4E-2</v>
       </c>
       <c r="I11" s="4">
         <f>H11*B11</f>
-        <v>0.42599999999999999</v>
+        <v>0.376</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="H12" s="4">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="I12" s="4">
+        <f>H12*B12</f>
+        <v>0.42599999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="4">
         <v>0.63100000000000001</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I13" s="4">
         <f t="shared" si="0"/>
         <v>1.262</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.246</v>
+      </c>
+      <c r="I14" s="4">
+        <f>H14*B14</f>
+        <v>0.246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0.09</v>
-      </c>
-      <c r="I13" s="4">
-        <f t="shared" si="0"/>
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="4">
+      <c r="F15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="4">
         <v>0.91800000000000004</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I15" s="4">
         <f t="shared" si="0"/>
         <v>1.8360000000000001</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.80400000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="8:10" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="4">
+        <f>SUM(I4:I16,I2)</f>
+        <v>21.981999999999996</v>
+      </c>
+    </row>
     <row r="20" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H20" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I20" s="4">
-        <f>SUM(I4:I14,I2)</f>
-        <v>20.727999999999998</v>
+        <f>I3</f>
+        <v>0.15</v>
       </c>
     </row>
     <row r="21" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H21" t="s">
         <v>53</v>
       </c>
-      <c r="I21" s="4">
-        <f>I3</f>
-        <v>0.15</v>
+      <c r="I21" s="8">
+        <f>I20+I19</f>
+        <v>22.131999999999994</v>
       </c>
     </row>
     <row r="22" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="H22" t="s">
-        <v>56</v>
-      </c>
-      <c r="I22" s="8">
-        <f>SUM(I2:I14)</f>
-        <v>20.878</v>
-      </c>
-    </row>
-    <row r="23" spans="8:10" x14ac:dyDescent="0.2">
-      <c r="J23" s="4"/>
+      <c r="J22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update with new CMS design and vertical RJ45
</commit_message>
<xml_diff>
--- a/iot2000/CAD/BOM.xlsx
+++ b/iot2000/CAD/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5720" yWindow="-19380" windowWidth="22640" windowHeight="12820" tabRatio="500"/>
+    <workbookView xWindow="11480" yWindow="-14480" windowWidth="29320" windowHeight="14140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
   <si>
     <t>Qté</t>
   </si>
@@ -110,9 +110,6 @@
     <t>1 M 5%</t>
   </si>
   <si>
-    <t>1.5KE27AHE3_A/C</t>
-  </si>
-  <si>
     <t>Suppresseur ESD  / diodes</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>504-EM366002</t>
   </si>
   <si>
-    <t>538-44620-0001</t>
-  </si>
-  <si>
     <t>FDS8958A-F085</t>
   </si>
   <si>
@@ -170,9 +164,6 @@
     <t>495-TSR2-2450</t>
   </si>
   <si>
-    <t>78-1.5KE27AHE3_A/C</t>
-  </si>
-  <si>
     <t>80-C315C102J3H9170TR</t>
   </si>
   <si>
@@ -267,6 +258,21 @@
   </si>
   <si>
     <t>R3, R4, R11, R12</t>
+  </si>
+  <si>
+    <t>538-95503-2881</t>
+  </si>
+  <si>
+    <t>95503-2881</t>
+  </si>
+  <si>
+    <t>SMAJ60A-TP</t>
+  </si>
+  <si>
+    <t>833-SMAJ60A-TP</t>
+  </si>
+  <si>
+    <t>MCC</t>
   </si>
 </sst>
 </file>
@@ -650,7 +656,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,16 +688,16 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -702,19 +708,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
       <c r="F2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
         <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>42</v>
       </c>
       <c r="H2" s="4">
         <v>0.46700000000000003</v>
@@ -732,19 +738,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H3">
         <v>0.15</v>
@@ -771,10 +777,10 @@
         <v>13</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="4">
         <v>1.23</v>
@@ -791,8 +797,8 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
-        <v>446200001</v>
+      <c r="C5" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="D5" t="s">
         <v>24</v>
@@ -801,10 +807,10 @@
         <v>23</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="H5" s="4">
         <v>0.68899999999999995</v>
@@ -822,7 +828,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -831,10 +837,10 @@
         <v>21</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H6" s="4">
         <v>0.76300000000000001</v>
@@ -861,10 +867,10 @@
         <v>10</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" s="4">
         <v>11.21</v>
@@ -882,26 +888,26 @@
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="H8" s="4">
-        <v>0.77900000000000003</v>
+        <v>0.51</v>
       </c>
       <c r="I8" s="4">
         <f t="shared" si="0"/>
-        <v>1.5580000000000001</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -912,19 +918,19 @@
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H9" s="4">
         <v>8.2000000000000003E-2</v>
@@ -942,19 +948,19 @@
         <v>2</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H10" s="15">
         <v>9.4E-2</v>
@@ -966,25 +972,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H11" s="17">
         <v>9.4E-2</v>
@@ -1002,19 +1008,19 @@
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H12" s="4">
         <v>0.21299999999999999</v>
@@ -1032,19 +1038,19 @@
         <v>2</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>31</v>
       </c>
-      <c r="E13" t="s">
-        <v>32</v>
-      </c>
       <c r="F13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H13" s="4">
         <v>0.63100000000000001</v>
@@ -1056,25 +1062,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H14" s="4">
         <v>0.246</v>
@@ -1086,25 +1092,25 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H15" s="4">
         <v>0.91800000000000004</v>
@@ -1116,25 +1122,25 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" t="s">
         <v>65</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" t="s">
-        <v>68</v>
       </c>
       <c r="H16" s="4">
         <v>0.80400000000000005</v>
@@ -1146,16 +1152,16 @@
     </row>
     <row r="19" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I19" s="4">
         <f>SUM(I4:I16,I2)</f>
-        <v>21.981999999999996</v>
+        <v>21.443999999999996</v>
       </c>
     </row>
     <row r="20" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I20" s="4">
         <f>I3</f>
@@ -1164,11 +1170,11 @@
     </row>
     <row r="21" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I21" s="8">
         <f>I20+I19</f>
-        <v>22.131999999999994</v>
+        <v>21.593999999999994</v>
       </c>
     </row>
     <row r="22" spans="8:10" x14ac:dyDescent="0.2">

</xml_diff>